<commit_message>
Updated API to v2.5.0. Resolved TSLint issues and npm audit issues.
</commit_message>
<xml_diff>
--- a/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\VennDiagram\14-9-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git1\documents\Published\Venn Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B989CC1-8B0C-476D-86A7-8497C8AD9E98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{87AE606C-9C12-4DEC-BB2E-96051D58853D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87AE606C-9C12-4DEC-BB2E-96051D58853D}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>S no</t>
   </si>
@@ -279,6 +280,18 @@
   </si>
   <si>
     <t>iPad - yes</t>
+  </si>
+  <si>
+    <t>Does visual legends stay in the same place when I filter data on my report?</t>
+  </si>
+  <si>
+    <t>null values</t>
+  </si>
+  <si>
+    <t>1. Drag null valued columns in Category and Measure field</t>
+  </si>
+  <si>
+    <t>Venn diagram should appear</t>
   </si>
 </sst>
 </file>
@@ -337,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -375,11 +388,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,22 +439,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD02BEF-CDC7-45AE-AEC8-BFE8DA79D8E7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +857,7 @@
       <c r="D5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -854,6 +893,23 @@
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D659F34-59B1-4B0D-984A-5AB844CFFE3F}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +953,7 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -908,10 +964,10 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -919,10 +975,10 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -930,10 +986,10 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -941,7 +997,7 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -952,10 +1008,10 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -963,10 +1019,10 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -974,10 +1030,10 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -985,10 +1041,10 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -996,10 +1052,10 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1007,10 +1063,10 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1018,7 +1074,7 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1029,7 +1085,7 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1040,10 +1096,10 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1051,10 +1107,10 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1087,10 +1143,10 @@
       <c r="A20" s="7">
         <v>17</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1098,7 +1154,7 @@
       <c r="A21" s="15">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -1107,26 +1163,26 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="10"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="16"/>
@@ -1135,10 +1191,10 @@
       <c r="A26" s="7">
         <v>19</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1146,10 +1202,21 @@
       <c r="A27" s="7">
         <v>20</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rendering Events API fixed
</commit_message>
<xml_diff>
--- a/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git1\documents\Published\Venn Diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Custom Visuals\SourceRepo\documents\Published\Venn Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B989CC1-8B0C-476D-86A7-8497C8AD9E98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C0C1F2-E9DF-463E-8AF6-EBE70BBC654C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87AE606C-9C12-4DEC-BB2E-96051D58853D}"/>
   </bookViews>
@@ -350,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -395,18 +395,9 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -414,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -442,12 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,9 +442,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,9 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD02BEF-CDC7-45AE-AEC8-BFE8DA79D8E7}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -806,13 +802,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -823,9 +819,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="4" t="s">
         <v>51</v>
       </c>
@@ -834,9 +830,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
@@ -896,19 +892,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>58</v>
       </c>
     </row>
@@ -927,9 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D659F34-59B1-4B0D-984A-5AB844CFFE3F}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1115,29 +1109,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -1151,41 +1145,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
@@ -1199,24 +1193,24 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="18">
         <v>20</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="20">
         <v>21</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="21" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>